<commit_message>
Completed the user login and access the feature.
</commit_message>
<xml_diff>
--- a/Dataset/RetailifyUserLoginAceessTable.xlsx
+++ b/Dataset/RetailifyUserLoginAceessTable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">UserID</t>
   </si>
@@ -72,6 +72,33 @@
   </si>
   <si>
     <t xml:space="preserve">alexnimbush999@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agrahari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agr123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agr@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agraalkll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jlkjlGu987978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agr1@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agrahari78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agshui87987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agr3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -553,6 +580,156 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1006</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>